<commit_message>
added remaining use cases
</commit_message>
<xml_diff>
--- a/documentation/TestCases.xlsx
+++ b/documentation/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Library/CloudStorage/GoogleDrive-stefan.bernhardsgruetter@redguard.ch/My Drive/sbernhardsgruetter/practice_lead_mobile_testing/MAS-Reference-App/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/code/MAS-Reference-App/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10939CE-0FFC-074C-A268-E267E929D2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27BDAF4-422A-8140-9738-CFFB0A59C626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{FCA74546-B262-594E-B9AE-410875231F12}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{FCA74546-B262-594E-B9AE-410875231F12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="173">
   <si>
     <t>MASVS-STORAGE</t>
   </si>
@@ -425,12 +425,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>DERECATED</t>
-  </si>
-  <si>
-    <t>TODO: Load Bouncy-Castle Keystroe</t>
-  </si>
-  <si>
     <t>N/A, because, we only test Default-Impementation</t>
   </si>
   <si>
@@ -461,15 +455,9 @@
     <t>TODO: Set up Server with Basic Auth</t>
   </si>
   <si>
-    <t>TODO: Implement HTTP-Server</t>
-  </si>
-  <si>
     <t>N/A beacause requires to develop own network-stack</t>
   </si>
   <si>
-    <t>TODO: Implement Server/</t>
-  </si>
-  <si>
     <t xml:space="preserve">TODO: Implement GOOD CASE  pinning using manifest, inline, webview, </t>
   </si>
   <si>
@@ -527,9 +515,6 @@
     <t>TODO: Obfuscate certain class</t>
   </si>
   <si>
-    <t>TODO: Obfuscate certain ressource</t>
-  </si>
-  <si>
     <t>????</t>
   </si>
   <si>
@@ -555,6 +540,21 @@
   </si>
   <si>
     <t>TODO: Access Device UUID</t>
+  </si>
+  <si>
+    <t>N/A (deprecated)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>TODO: Implement HTTP Server</t>
+  </si>
+  <si>
+    <t>TODO: Implement SIP/RTP</t>
+  </si>
+  <si>
+    <t>N/A because not part of Android</t>
   </si>
 </sst>
 </file>
@@ -749,7 +749,18 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1095,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC40AF35-D4A9-2F49-881F-BB4592B4F7A9}">
   <dimension ref="A1:C125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="B125" sqref="B125"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1225,7 +1236,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1241,7 +1252,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1273,7 +1284,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1350,7 +1361,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1358,7 +1369,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1366,7 +1377,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1382,10 +1393,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C36" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1393,7 +1404,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1401,7 +1412,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1409,7 +1420,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1417,7 +1428,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1425,7 +1436,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1433,7 +1444,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1441,7 +1452,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1449,7 +1460,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+      <c r="C44" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1457,7 +1471,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1465,7 +1479,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1473,7 +1487,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1484,7 +1498,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:3">
       <c r="A49" s="6" t="s">
         <v>47</v>
       </c>
@@ -1492,113 +1506,134 @@
         <v>126</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:3">
       <c r="A50" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:3">
       <c r="A52" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>140</v>
+      </c>
+      <c r="C52" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" s="8" t="s">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>171</v>
+      </c>
+      <c r="C53" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>170</v>
+      </c>
+      <c r="C55" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+        <v>141</v>
+      </c>
+      <c r="C56" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
+        <v>142</v>
+      </c>
+      <c r="C57" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:3">
       <c r="A59" s="10" t="s">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+        <v>145</v>
+      </c>
+      <c r="C60" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <v>144</v>
+      </c>
+      <c r="C61" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" s="10" t="s">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="10" t="s">
         <v>62</v>
       </c>
@@ -1606,31 +1641,34 @@
         <v>126</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:3">
       <c r="A65" s="10" t="s">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+        <v>147</v>
+      </c>
+      <c r="C65" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="10" t="s">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="10" t="s">
         <v>66</v>
       </c>
@@ -1638,7 +1676,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:3">
       <c r="A69" s="10" t="s">
         <v>67</v>
       </c>
@@ -1646,7 +1684,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:3">
       <c r="A70" s="10" t="s">
         <v>68</v>
       </c>
@@ -1654,7 +1692,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:3">
       <c r="A71" s="10" t="s">
         <v>69</v>
       </c>
@@ -1662,7 +1700,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:3">
       <c r="A72" s="10" t="s">
         <v>70</v>
       </c>
@@ -1670,15 +1708,15 @@
         <v>126</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:3">
       <c r="A73" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="10" t="s">
         <v>72</v>
       </c>
@@ -1686,7 +1724,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:3">
       <c r="A75" s="10" t="s">
         <v>73</v>
       </c>
@@ -1694,7 +1732,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:3">
       <c r="A76" s="10" t="s">
         <v>74</v>
       </c>
@@ -1702,7 +1740,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:3">
       <c r="A77" s="10" t="s">
         <v>75</v>
       </c>
@@ -1710,68 +1748,80 @@
         <v>126</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:3">
       <c r="A78" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="17">
       <c r="A79" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" s="10" t="s">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
+        <v>148</v>
+      </c>
+      <c r="C80" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="A81" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:3">
       <c r="A82" s="12" t="s">
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
+        <v>152</v>
+      </c>
+      <c r="C82" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83" s="12" t="s">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
+        <v>153</v>
+      </c>
+      <c r="C83" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" s="12" t="s">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
+        <v>154</v>
+      </c>
+      <c r="C84" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" s="12" t="s">
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" s="12" t="s">
         <v>84</v>
       </c>
@@ -1779,7 +1829,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:3">
       <c r="A87" s="12" t="s">
         <v>85</v>
       </c>
@@ -1787,7 +1837,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:3">
       <c r="A88" s="12" t="s">
         <v>86</v>
       </c>
@@ -1795,7 +1845,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:3">
       <c r="A89" s="12" t="s">
         <v>87</v>
       </c>
@@ -1803,7 +1853,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:3">
       <c r="A90" s="12" t="s">
         <v>88</v>
       </c>
@@ -1811,7 +1861,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:3">
       <c r="A91" s="12" t="s">
         <v>89</v>
       </c>
@@ -1819,7 +1869,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:3">
       <c r="A92" s="12" t="s">
         <v>90</v>
       </c>
@@ -1827,116 +1877,134 @@
         <v>128</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:3">
       <c r="A93" s="12" t="s">
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
+        <v>155</v>
+      </c>
+      <c r="C93" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
       <c r="A94" s="12" t="s">
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
+        <v>156</v>
+      </c>
+      <c r="C94" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
       <c r="A95" s="12" t="s">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
+        <v>157</v>
+      </c>
+      <c r="C95" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
       <c r="A96" s="12" t="s">
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:3">
       <c r="A98" s="14" t="s">
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
+        <v>158</v>
+      </c>
+      <c r="C98" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" s="14" t="s">
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100" s="14" t="s">
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
+        <v>160</v>
+      </c>
+      <c r="C102" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" s="14" t="s">
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" s="14" t="s">
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" s="14" t="s">
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" s="14" t="s">
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
+        <v>162</v>
+      </c>
+      <c r="C106" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" s="14" t="s">
         <v>105</v>
       </c>
@@ -1944,7 +2012,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:3">
       <c r="A108" s="14" t="s">
         <v>106</v>
       </c>
@@ -1952,15 +2020,15 @@
         <v>126</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:3">
       <c r="A109" s="14" t="s">
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" s="14" t="s">
         <v>108</v>
       </c>
@@ -1968,20 +2036,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:3">
       <c r="A111" s="14" t="s">
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
       <c r="A112" s="14" t="s">
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1989,7 +2057,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1997,7 +2065,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2005,7 +2073,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2013,7 +2081,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2026,7 +2094,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2034,7 +2102,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2042,7 +2110,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2050,7 +2118,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2058,7 +2126,7 @@
         <v>120</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2066,7 +2134,7 @@
         <v>121</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2074,7 +2142,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2082,10 +2150,15 @@
         <v>123</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B125">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TODO:">
+      <formula>NOT(ISERROR(SEARCH("TODO:",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="https://mas.owasp.org/MASWE/MASVS-STORAGE/MASWE-0001/" xr:uid="{B6CB61CA-1E38-0541-8AC7-04096F90CB5D}"/>
     <hyperlink ref="A4" r:id="rId2" display="https://mas.owasp.org/MASWE/MASVS-STORAGE/MASWE-0002/" xr:uid="{FB9557FC-630C-5447-89BA-E81EBDA5BD92}"/>

</xml_diff>

<commit_message>
added additional use cases
</commit_message>
<xml_diff>
--- a/documentation/TestCases.xlsx
+++ b/documentation/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/code/MAS-Reference-App/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDC0874-953C-B24B-A34C-6131A981F6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A7E6A4-2F43-5F43-95F2-22F1A78E224C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{FCA74546-B262-594E-B9AE-410875231F12}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="164">
   <si>
     <t>MASVS-STORAGE</t>
   </si>
@@ -464,18 +464,9 @@
     <t>N/A beacause it is too broad</t>
   </si>
   <si>
-    <t>TODO: manually block screenshots taking for views</t>
-  </si>
-  <si>
-    <t>TODO: send sensitvie data to notifications</t>
-  </si>
-  <si>
     <t>N/A (mabey TODO later)</t>
   </si>
   <si>
-    <t>TODO: use localhost for IPC</t>
-  </si>
-  <si>
     <t>TODO: not using WebViewAssetLoader</t>
   </si>
   <si>
@@ -485,15 +476,9 @@
     <t>N/A beacause part of Manifest</t>
   </si>
   <si>
-    <t>TODO: AppUpdateManager Test</t>
-  </si>
-  <si>
     <t>TODO: Add SDK and Web-Library with KNOWN vulnerabilities</t>
   </si>
   <si>
-    <t>TODO: Get Platform-Version</t>
-  </si>
-  <si>
     <t>TODO: SQL-Injection using local SQLite</t>
   </si>
   <si>
@@ -528,9 +513,6 @@
   </si>
   <si>
     <t>N/A because not a technical requirement</t>
-  </si>
-  <si>
-    <t>TODO: Access Device UUID</t>
   </si>
   <si>
     <t>N/A (deprecated)</t>
@@ -1097,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC40AF35-D4A9-2F49-881F-BB4592B4F7A9}">
   <dimension ref="A1:C125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1227,7 +1209,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1515,7 +1497,7 @@
         <v>139</v>
       </c>
       <c r="C52" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1523,10 +1505,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C53" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1542,10 +1524,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C55" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1556,7 +1538,7 @@
         <v>140</v>
       </c>
       <c r="C56" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1577,7 +1559,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1585,10 +1567,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="C60" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1596,10 +1578,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C61" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1607,7 +1589,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1615,7 +1597,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1631,10 +1613,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="C65" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1642,7 +1624,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1650,7 +1632,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1698,7 +1680,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1738,7 +1720,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17">
@@ -1746,7 +1728,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1756,9 +1738,6 @@
       <c r="B80" t="s">
         <v>126</v>
       </c>
-      <c r="C80" t="s">
-        <v>166</v>
-      </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="11" t="s">
@@ -1770,10 +1749,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="C82" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1781,10 +1760,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C83" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1792,10 +1771,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="C84" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1803,7 +1782,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1867,10 +1846,10 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C93" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1878,10 +1857,10 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C94" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1889,10 +1868,10 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C95" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1900,7 +1879,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1913,10 +1892,10 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C98" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1924,7 +1903,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1932,7 +1911,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1940,7 +1919,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1948,10 +1927,10 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C102" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1959,7 +1938,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1983,10 +1962,10 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C106" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2010,10 +1989,10 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
+        <v>155</v>
+      </c>
+      <c r="C109" t="s">
         <v>160</v>
-      </c>
-      <c r="C109" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2029,10 +2008,10 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C111" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2040,7 +2019,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2048,10 +2027,10 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
+        <v>155</v>
+      </c>
+      <c r="C113" t="s">
         <v>160</v>
-      </c>
-      <c r="C113" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2059,7 +2038,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2067,7 +2046,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2075,7 +2054,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2104,10 +2083,10 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="C120" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2115,7 +2094,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2123,7 +2102,7 @@
         <v>120</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2131,7 +2110,7 @@
         <v>121</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2139,7 +2118,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2147,7 +2126,7 @@
         <v>123</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>